<commit_message>
Regenerated all IGs after many changes to all STU3 profiles.
</commit_message>
<xml_diff>
--- a/output/PrescriptionDispenseLists/device-dh-base-1.xlsx
+++ b/output/PrescriptionDispenseLists/device-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="338">
   <si>
     <t>Path</t>
   </si>
@@ -863,7 +863,13 @@
     <t>Code or identifier to identify a kind of device.</t>
   </si>
   <si>
-    <t>Codes to identify medical devices.</t>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes to identify medical devices</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/device-kind</t>
   </si>
   <si>
     <t>.code</t>
@@ -1077,9 +1083,6 @@
   </si>
   <si>
     <t>Provides additional safety characteristics about a medical device.  For example devices containing latex.</t>
-  </si>
-  <si>
-    <t>example</t>
   </si>
   <si>
     <t>Codes used to identify medical devices safety characterics. These codes are derived in part from the [United States Food and Drug Administration recommendations](http://www.fda.gov/downloads/medicaldevices/deviceregulationandguidance/guidancedocuments/ucm107708.pdf) and are provided here as a suggestive example.</t>
@@ -5229,13 +5232,13 @@
         <v>39</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>70</v>
+        <v>264</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>39</v>
+        <v>266</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>39</v>
@@ -5268,18 +5271,18 @@
         <v>39</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>213</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5305,10 +5308,10 @@
         <v>118</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5359,7 +5362,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5374,18 +5377,18 @@
         <v>39</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>213</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5411,10 +5414,10 @@
         <v>118</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5465,7 +5468,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5480,7 +5483,7 @@
         <v>39</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>213</v>
@@ -5491,7 +5494,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5514,13 +5517,13 @@
         <v>39</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5571,7 +5574,7 @@
         <v>39</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5586,18 +5589,18 @@
         <v>39</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>213</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5620,13 +5623,13 @@
         <v>39</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -5677,7 +5680,7 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -5692,18 +5695,18 @@
         <v>39</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>213</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5729,10 +5732,10 @@
         <v>118</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -5783,7 +5786,7 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
@@ -5798,7 +5801,7 @@
         <v>39</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>213</v>
@@ -5809,7 +5812,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5835,10 +5838,10 @@
         <v>118</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -5889,7 +5892,7 @@
         <v>39</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>40</v>
@@ -5904,7 +5907,7 @@
         <v>39</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>213</v>
@@ -5915,7 +5918,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5938,17 +5941,17 @@
         <v>39</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>39</v>
@@ -5997,7 +6000,7 @@
         <v>39</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>40</v>
@@ -6012,10 +6015,10 @@
         <v>39</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>39</v>
@@ -6023,7 +6026,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6046,13 +6049,13 @@
         <v>39</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6103,7 +6106,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6118,10 +6121,10 @@
         <v>39</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>39</v>
@@ -6129,7 +6132,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6152,16 +6155,16 @@
         <v>39</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6211,7 +6214,7 @@
         <v>39</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
@@ -6226,10 +6229,10 @@
         <v>39</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>39</v>
@@ -6237,7 +6240,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6260,17 +6263,17 @@
         <v>39</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>39</v>
@@ -6319,7 +6322,7 @@
         <v>39</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6334,10 +6337,10 @@
         <v>39</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>39</v>
@@ -6345,7 +6348,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6371,13 +6374,13 @@
         <v>60</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6427,7 +6430,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6442,10 +6445,10 @@
         <v>39</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>39</v>
@@ -6453,7 +6456,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6476,13 +6479,13 @@
         <v>39</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6533,7 +6536,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6548,7 +6551,7 @@
         <v>39</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>39</v>
@@ -6559,7 +6562,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6585,10 +6588,10 @@
         <v>139</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6615,13 +6618,13 @@
         <v>39</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>334</v>
+        <v>264</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>39</v>
@@ -6639,7 +6642,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>

</xml_diff>

<commit_message>
Updated output of all IG's following changes to intro.md's and known issues (IG's and profiles).
</commit_message>
<xml_diff>
--- a/output/PrescriptionDispenseLists/device-dh-base-1.xlsx
+++ b/output/PrescriptionDispenseLists/device-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="338">
   <si>
     <t>Path</t>
   </si>
@@ -863,7 +863,13 @@
     <t>Code or identifier to identify a kind of device.</t>
   </si>
   <si>
-    <t>Codes to identify medical devices.</t>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes to identify medical devices</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/device-kind</t>
   </si>
   <si>
     <t>.code</t>
@@ -1077,9 +1083,6 @@
   </si>
   <si>
     <t>Provides additional safety characteristics about a medical device.  For example devices containing latex.</t>
-  </si>
-  <si>
-    <t>example</t>
   </si>
   <si>
     <t>Codes used to identify medical devices safety characterics. These codes are derived in part from the [United States Food and Drug Administration recommendations](http://www.fda.gov/downloads/medicaldevices/deviceregulationandguidance/guidancedocuments/ucm107708.pdf) and are provided here as a suggestive example.</t>
@@ -5229,13 +5232,13 @@
         <v>39</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>70</v>
+        <v>264</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>39</v>
+        <v>266</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>39</v>
@@ -5268,18 +5271,18 @@
         <v>39</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>213</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5305,10 +5308,10 @@
         <v>118</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5359,7 +5362,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5374,18 +5377,18 @@
         <v>39</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>213</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5411,10 +5414,10 @@
         <v>118</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5465,7 +5468,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5480,7 +5483,7 @@
         <v>39</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>213</v>
@@ -5491,7 +5494,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5514,13 +5517,13 @@
         <v>39</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5571,7 +5574,7 @@
         <v>39</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5586,18 +5589,18 @@
         <v>39</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>213</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5620,13 +5623,13 @@
         <v>39</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -5677,7 +5680,7 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -5692,18 +5695,18 @@
         <v>39</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>213</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5729,10 +5732,10 @@
         <v>118</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -5783,7 +5786,7 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
@@ -5798,7 +5801,7 @@
         <v>39</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>213</v>
@@ -5809,7 +5812,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5835,10 +5838,10 @@
         <v>118</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -5889,7 +5892,7 @@
         <v>39</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>40</v>
@@ -5904,7 +5907,7 @@
         <v>39</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>213</v>
@@ -5915,7 +5918,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5938,17 +5941,17 @@
         <v>39</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>39</v>
@@ -5997,7 +6000,7 @@
         <v>39</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>40</v>
@@ -6012,10 +6015,10 @@
         <v>39</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>39</v>
@@ -6023,7 +6026,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6046,13 +6049,13 @@
         <v>39</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6103,7 +6106,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6118,10 +6121,10 @@
         <v>39</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>39</v>
@@ -6129,7 +6132,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6152,16 +6155,16 @@
         <v>39</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6211,7 +6214,7 @@
         <v>39</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
@@ -6226,10 +6229,10 @@
         <v>39</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>39</v>
@@ -6237,7 +6240,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6260,17 +6263,17 @@
         <v>39</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>39</v>
@@ -6319,7 +6322,7 @@
         <v>39</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6334,10 +6337,10 @@
         <v>39</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>39</v>
@@ -6345,7 +6348,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6371,13 +6374,13 @@
         <v>60</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -6427,7 +6430,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6442,10 +6445,10 @@
         <v>39</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>39</v>
@@ -6453,7 +6456,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6476,13 +6479,13 @@
         <v>39</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6533,7 +6536,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6548,7 +6551,7 @@
         <v>39</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>39</v>
@@ -6559,7 +6562,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6585,10 +6588,10 @@
         <v>139</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6615,13 +6618,13 @@
         <v>39</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>334</v>
+        <v>264</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>39</v>
@@ -6639,7 +6642,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>

</xml_diff>